<commit_message>
added safety breach check
</commit_message>
<xml_diff>
--- a/excel/shanRoyale2022Data1.xlsx
+++ b/excel/shanRoyale2022Data1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Casper/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prave\Desktop\tech-projects\medium-projects\telegram-bot\shan-royale-2022\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0489A34C-F58C-3241-97EF-9F26014E6248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DB22DD-3691-4240-BAA3-3FAE769CEFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{052D59D5-69DE-493C-8002-AE6F997C54F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{052D59D5-69DE-493C-8002-AE6F997C54F8}"/>
   </bookViews>
   <sheets>
     <sheet name="playerDataRound1" sheetId="1" r:id="rId1"/>
@@ -466,15 +466,15 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="11" width="13.83203125" style="1" customWidth="1"/>
+    <col min="1" max="11" width="13.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -544,7 +544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -658,16 +658,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EAB414-4D8E-4715-81F5-BB9EBEC690BA}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="11" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,7 +702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -851,16 +851,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B16F35-1C91-4BD6-99C6-D356DCD5059C}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="19.6640625" style="2" customWidth="1"/>
+    <col min="1" max="5" width="19.6328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -877,7 +877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -928,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
right and wrong kill handlers
</commit_message>
<xml_diff>
--- a/excel/shanRoyale2022Data1.xlsx
+++ b/excel/shanRoyale2022Data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prave\Desktop\tech-projects\medium-projects\telegram-bot\shan-royale-2022\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D39D125-2B4D-4365-95A0-21B5A1BF2D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306BD68B-A94C-406A-96B4-D9864A36AED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{052D59D5-69DE-493C-8002-AE6F997C54F8}"/>
+    <workbookView xWindow="-27660" yWindow="1140" windowWidth="21600" windowHeight="11175" xr2:uid="{052D59D5-69DE-493C-8002-AE6F997C54F8}"/>
   </bookViews>
   <sheets>
     <sheet name="playerDataRound1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,10 +587,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
         <v>70</v>

</xml_diff>